<commit_message>
Accomplish PDF download - first try
</commit_message>
<xml_diff>
--- a/recipients.xlsx
+++ b/recipients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cristina_Lazarte_4-2-25.pdf</t>
+          <t>Pdf_de_prueba.pdf</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -517,27 +517,49 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Micaela</t>
+          <t>Matias</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>micaela@email.com</t>
+          <t>matiasmalleville@gmail.com</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Micaela_Payment.pdf</t>
+          <t>Matias Malleville.pdf</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Pablo</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>roig@lacaja.com.ar</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pablo Roig.pdf</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>

</xml_diff>